<commit_message>
Pequenos acertos na conversão para PageObjectFactory
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.santos\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.santos\Documents\Massa de dados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B07A00C-B2A0-4E68-B22F-BF0AAF65B07E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3AE9B2-3B4B-4110-9E48-2E1C6CC3CF04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="-2175" windowWidth="24240" windowHeight="13140" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
@@ -66,9 +66,6 @@
     <t>CEP</t>
   </si>
   <si>
-    <t>DrGus</t>
-  </si>
-  <si>
     <t>Gus123@</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>12345-678</t>
+  </si>
+  <si>
+    <t>Deusstsvs</t>
   </si>
 </sst>
 </file>
@@ -510,12 +510,12 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
@@ -566,37 +566,37 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>20</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Aperfeiçoamento do código em page object factory
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.santos\Documents\Massa de dados\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3AE9B2-3B4B-4110-9E48-2E1C6CC3CF04}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{48E5A37B-53F3-4946-B089-4B36A84B89AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="-2175" windowWidth="24240" windowHeight="13140" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
   <sheets>
-    <sheet name="cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="CenariosDeTeste" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
   <si>
     <t>Username</t>
   </si>
@@ -97,6 +93,42 @@
   </si>
   <si>
     <t>Deusstsvs</t>
+  </si>
+  <si>
+    <t>Cenario</t>
+  </si>
+  <si>
+    <t>Cadastro</t>
+  </si>
+  <si>
+    <t>Buscar Produto</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>Tipo de Produto</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Positivo/Negativo</t>
+  </si>
+  <si>
+    <t>Nome do Produto</t>
+  </si>
+  <si>
+    <t>HP USB 3 BUTTON OPTICAL MOUSE</t>
+  </si>
+  <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>Negativo</t>
+  </si>
+  <si>
+    <t>mouse hp</t>
   </si>
 </sst>
 </file>
@@ -507,108 +539,164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C2567E2-D904-4AF5-AA09-5D36B24D5ECF}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="6"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E7" s="1"/>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K8" s="6"/>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="D7" s="1"/>
+      <c r="G7" s="1"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{1C085938-D071-4401-8162-D1354893ADAF}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{A6769731-262F-4251-B429-6AA05E7FA330}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{1C085938-D071-4401-8162-D1354893ADAF}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{A6769731-262F-4251-B429-6AA05E7FA330}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>

<commit_message>
Refatorando algumas classes e reajustando screenshotd
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{48E5A37B-53F3-4946-B089-4B36A84B89AC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\g.santos\eclipse-workspace\ProjetoTDD\src\main\java\br\com\rsinet\hub_tdd\dadosParaTeste\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417DAD1D-2FD7-4A7E-B027-9D170A134C64}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
   <sheets>
     <sheet name="CenariosDeTeste" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -92,9 +90,6 @@
     <t>12345-678</t>
   </si>
   <si>
-    <t>Deusstsvs</t>
-  </si>
-  <si>
     <t>Cenario</t>
   </si>
   <si>
@@ -129,6 +124,9 @@
   </si>
   <si>
     <t>mouse hp</t>
+  </si>
+  <si>
+    <t>UsuarioNovo</t>
   </si>
 </sst>
 </file>
@@ -542,7 +540,7 @@
   <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +562,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
@@ -605,13 +603,13 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>11</v>
@@ -646,44 +644,44 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="D5" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Envio de arquivos remanescentes
</commit_message>
<xml_diff>
--- a/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
+++ b/src/main/java/br/com/rsinet/hub_tdd/dadosParaTeste/DadosParaTeste.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\TDD\src\main\java\br\com\rsinet\hub_tdd\dadosParaTeste\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Workspace\ProjetoTDD\src\main\java\br\com\rsinet\hub_tdd\dadosParaTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{021A9BB5-7C25-4BB0-A14E-1D7A615DFBB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DA1829-2A79-40C5-85F2-15AF9E91C299}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="15375" windowHeight="7875" xr2:uid="{AACC88D3-5814-4D61-8B68-BC0AA92C6385}"/>
   </bookViews>
   <sheets>
     <sheet name="CenariosDeTeste" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
     <t>mouse hp</t>
   </si>
   <si>
-    <t>piwpfkna</t>
+    <t>muarara</t>
   </si>
 </sst>
 </file>

</xml_diff>